<commit_message>
Updated slot card functionality test data
</commit_message>
<xml_diff>
--- a/Test Data/TC_40_Verify_Node_Selection_In_Project_View_On_Addition_Of_Slot_Loop_Cards.xlsx
+++ b/Test Data/TC_40_Verify_Node_Selection_In_Project_View_On_Addition_Of_Slot_Loop_Cards.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E63AB65-77A2-4B5F-A416-BC7A6FF8EC4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices" sheetId="6" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Add Devices for Second Panel" sheetId="8" r:id="rId3"/>
     <sheet name="Delete Devices for Second Panel" sheetId="9" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -135,9 +134,6 @@
     <t>FB800</t>
   </si>
   <si>
-    <t>PCH800</t>
-  </si>
-  <si>
     <t>Other Slot card name</t>
   </si>
   <si>
@@ -147,9 +143,6 @@
     <t>Label Name</t>
   </si>
   <si>
-    <t>PCH800-1</t>
-  </si>
-  <si>
     <t>Other Slot Cards Name</t>
   </si>
   <si>
@@ -165,19 +158,25 @@
     <t>Pro32xBB</t>
   </si>
   <si>
-    <t>PCH800-2</t>
-  </si>
-  <si>
     <t>Other Slot Cards  (1 of 18)</t>
   </si>
   <si>
     <t>Other Slot Cards  (2 of 18)</t>
+  </si>
+  <si>
+    <t>PCH800 5.0A</t>
+  </si>
+  <si>
+    <t>PCH800 5.0A-1</t>
+  </si>
+  <si>
+    <t>PCH800 5.0A-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,11 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:J11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +617,7 @@
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -644,7 +643,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>0</v>
@@ -663,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
@@ -681,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
@@ -748,7 +747,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>9</v>
@@ -757,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>13</v>
@@ -857,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>15</v>
@@ -869,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>20</v>
@@ -919,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O11" s="14" t="s">
         <v>20</v>
@@ -938,11 +937,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BF4F55-E4E9-4F29-A723-2FD2D613116E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,7 +949,7 @@
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -973,7 +972,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>0</v>
@@ -985,7 +984,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
@@ -997,7 +996,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
@@ -1047,10 +1046,10 @@
         <v>24</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>20</v>
@@ -1082,7 +1081,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>31</v>
@@ -1097,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>20</v>
@@ -1116,11 +1115,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF82D6F5-1363-425F-A4FD-116ADB5A1545}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1130,7 @@
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -1157,7 +1156,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>0</v>
@@ -1176,7 +1175,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
@@ -1194,7 +1193,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
@@ -1261,7 +1260,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>9</v>
@@ -1270,7 +1269,7 @@
         <v>16</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>13</v>
@@ -1343,7 +1342,7 @@
     </row>
     <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>26</v>
@@ -1370,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>15</v>
@@ -1382,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O10" s="14" t="s">
         <v>20</v>
@@ -1432,7 +1431,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O11" s="14" t="s">
         <v>20</v>
@@ -1451,11 +1450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5046C648-E650-487F-A70A-BBBA83CD8585}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1463,7 +1462,7 @@
     <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -1486,7 +1485,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>0</v>
@@ -1498,7 +1497,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
@@ -1510,7 +1509,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
@@ -1560,10 +1559,10 @@
         <v>24</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>20</v>
@@ -1586,7 +1585,7 @@
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>26</v>
@@ -1595,7 +1594,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>31</v>
@@ -1610,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>20</v>

</xml_diff>